<commit_message>
Ajout d'un fichier excel du temps passé par chaque membre et pour chaque tache du projet
</commit_message>
<xml_diff>
--- a/Rapport/TpsParPersonne.xlsx
+++ b/Rapport/TpsParPersonne.xlsx
@@ -70,7 +70,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +95,22 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -192,20 +208,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -214,6 +218,26 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -514,7 +538,7 @@
   <dimension ref="D2:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -522,190 +546,190 @@
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:12" ht="23.4">
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
-    </row>
-    <row r="5" spans="4:12">
-      <c r="D5" s="5"/>
-      <c r="E5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="5" spans="4:12" s="11" customFormat="1" ht="31.2" customHeight="1">
+      <c r="D5" s="10"/>
+      <c r="E5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="4:12">
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4">
         <f>SUM(E6:K6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="4:12">
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4">
         <f t="shared" ref="L7:L13" si="0">SUM(E7:K7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="4:12">
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5">
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="4:12">
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="4:12">
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5">
+      <c r="E10" s="8"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="4:12">
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="4:12">
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="4:12">
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <f>SUM(E6:E12)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="5">
-        <f t="shared" ref="F13:L13" si="1">SUM(F6:F12)</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="5">
+      <c r="F13" s="4">
+        <f t="shared" ref="F13:K13" si="1">SUM(F6:F12)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Ajouts d'elements au rapport.
</commit_message>
<xml_diff>
--- a/Rapport/TpsParPersonne.xlsx
+++ b/Rapport/TpsParPersonne.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="22116" windowHeight="9528"/>
@@ -11,7 +11,7 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -69,8 +69,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,15 +210,6 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -238,6 +229,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -247,6 +247,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -325,6 +330,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -359,6 +365,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -534,14 +541,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
@@ -550,188 +557,202 @@
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:12" ht="23.4">
-      <c r="E2" s="1" t="s">
+    <row r="2" spans="4:12" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="E2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="5" spans="4:12" s="11" customFormat="1" ht="31.2" customHeight="1">
-      <c r="D5" s="10"/>
-      <c r="E5" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="9" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="5" spans="4:12" s="8" customFormat="1" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="7"/>
+      <c r="E5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="4:12">
-      <c r="D6" s="5" t="s">
+    <row r="6" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1">
         <f>SUM(E6:K6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="4:12">
-      <c r="D7" s="5" t="s">
+    <row r="7" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1">
         <f t="shared" ref="L7:L13" si="0">SUM(E7:K7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="4:12">
-      <c r="D8" s="6" t="s">
+    <row r="8" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4">
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>18</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1">
+        <v>6</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="4:12">
-      <c r="D9" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="4:12">
-      <c r="D10" s="7" t="s">
+    <row r="10" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4">
+      <c r="E10" s="5"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="4:12">
-      <c r="D11" s="7" t="s">
+    <row r="11" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="4:12">
-      <c r="D12" s="7" t="s">
+    <row r="12" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="4:12">
-      <c r="D13" s="7" t="s">
+    <row r="13" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="1">
         <f>SUM(E6:E12)</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="4">
+        <v>5</v>
+      </c>
+      <c r="F13" s="1">
         <f t="shared" ref="F13:K13" si="1">SUM(F6:F12)</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="4">
+        <v>5</v>
+      </c>
+      <c r="G13" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="4">
+        <v>18</v>
+      </c>
+      <c r="H13" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="4">
+        <v>5</v>
+      </c>
+      <c r="J13" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="4">
+        <v>6</v>
+      </c>
+      <c r="K13" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="4">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -744,24 +765,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout temps par personne
</commit_message>
<xml_diff>
--- a/Rapport/TpsParPersonne.xlsx
+++ b/Rapport/TpsParPersonne.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mon boulot\OO-Livraisons\Rapport\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="22116" windowHeight="9528"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="22110" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve">Capture et analyse des besoins </t>
   </si>
@@ -25,9 +30,6 @@
   </si>
   <si>
     <t>Impléméntation du code du prototype</t>
-  </si>
-  <si>
-    <t>Code IHM</t>
   </si>
   <si>
     <t>Tests</t>
@@ -142,7 +144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -189,26 +191,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -236,9 +225,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20 % - Accent1" xfId="2" builtinId="30"/>
@@ -250,6 +236,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -298,7 +287,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -333,7 +322,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -542,30 +531,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:L13"/>
+  <dimension ref="D2:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:12" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="4:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="E2" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="5" spans="4:12" s="8" customFormat="1" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="4:11" s="8" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="7"/>
       <c r="E5" s="6" t="s">
         <v>0</v>
@@ -586,77 +574,91 @@
         <v>5</v>
       </c>
       <c r="K5" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="1">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>40</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1">
+        <v>4</v>
+      </c>
+      <c r="K6" s="1">
+        <f>SUM(E6:J6)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1">
-        <f>SUM(E6:K6)</f>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>45</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D7" s="2" t="s">
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <f>SUM(E7:J7)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1">
-        <f t="shared" ref="L7:L13" si="0">SUM(E7:K7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D8" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="E8" s="1">
         <v>5</v>
       </c>
       <c r="F8" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1">
         <v>18</v>
       </c>
       <c r="H8" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I8" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J8" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K8" s="1">
-        <v>1</v>
-      </c>
-      <c r="L8" s="1">
-        <f t="shared" si="0"/>
+        <f>SUM(E8:J8)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -664,15 +666,14 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1">
-        <f t="shared" si="0"/>
+      <c r="K9" s="1">
+        <f>SUM(E9:J9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="1"/>
@@ -680,15 +681,14 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1">
-        <f t="shared" si="0"/>
+      <c r="K10" s="1">
+        <f>SUM(E10:J10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D11" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -696,15 +696,14 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1">
-        <f t="shared" si="0"/>
+      <c r="K11" s="1">
+        <f>SUM(E11:J11)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D12" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -712,52 +711,47 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1">
-        <f t="shared" si="0"/>
+      <c r="K12" s="1">
+        <f>SUM(E12:J12)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1">
         <f>SUM(E6:E12)</f>
+        <v>15</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" ref="F13:J13" si="0">SUM(F6:F12)</f>
+        <v>19</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F13" s="1">
-        <f t="shared" ref="F13:K13" si="1">SUM(F6:F12)</f>
-        <v>5</v>
-      </c>
-      <c r="G13" s="1">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="H13" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="J13" s="1">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
       <c r="K13" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L13" s="1">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>SUM(E13:J13)</f>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
@@ -770,7 +764,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -782,7 +776,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout du rappport modifié par Mohamme
</commit_message>
<xml_diff>
--- a/Rapport/TpsParPersonne.xlsx
+++ b/Rapport/TpsParPersonne.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mon boulot\OO-Livraisons\Rapport\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="22110" windowHeight="9525"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="22116" windowHeight="9528"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -71,8 +66,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,7 +192,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -205,9 +200,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -287,7 +279,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -319,10 +311,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -354,7 +345,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -530,54 +520,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E2" s="9" t="s">
+    <row r="2" spans="4:11" ht="23.4">
+      <c r="E2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="5" spans="4:11" s="8" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="7"/>
-      <c r="E5" s="6" t="s">
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="5" spans="4:11" s="7" customFormat="1" ht="31.2" customHeight="1">
+      <c r="D5" s="6"/>
+      <c r="E5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:11">
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
@@ -598,11 +588,11 @@
         <v>4</v>
       </c>
       <c r="K6" s="1">
-        <f>SUM(E6:J6)</f>
+        <f t="shared" ref="K6:K13" si="0">SUM(E6:J6)</f>
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:11">
       <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
@@ -625,11 +615,11 @@
         <v>0</v>
       </c>
       <c r="K7" s="1">
-        <f>SUM(E7:J7)</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:11">
       <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
@@ -652,41 +642,65 @@
         <v>1</v>
       </c>
       <c r="K8" s="1">
-        <f>SUM(E8:J8)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:11">
       <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="E9" s="1">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1">
+        <v>9</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2</v>
+      </c>
       <c r="K9" s="1">
-        <f>SUM(E9:J9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="4:11">
       <c r="D10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="E10" s="1">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1">
+        <v>12</v>
+      </c>
+      <c r="I10" s="1">
+        <v>6</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.5</v>
+      </c>
       <c r="K10" s="1">
-        <f>SUM(E10:J10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11">
       <c r="D11" s="4" t="s">
         <v>9</v>
       </c>
@@ -697,56 +711,68 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1">
-        <f>SUM(E11:J11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:11">
       <c r="D12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="E12" s="1">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1">
+        <v>7</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
       <c r="K12" s="1">
-        <f>SUM(E12:J12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11">
       <c r="D13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="1">
         <f>SUM(E6:E12)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" ref="F13:J13" si="0">SUM(F6:F12)</f>
-        <v>19</v>
+        <f t="shared" ref="F13:J13" si="1">SUM(F6:F12)</f>
+        <v>41</v>
       </c>
       <c r="G13" s="1">
+        <f t="shared" si="1"/>
+        <v>153</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="K13" s="1">
         <f t="shared" si="0"/>
-        <v>103</v>
-      </c>
-      <c r="H13" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="I13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J13" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="K13" s="1">
-        <f>SUM(E13:J13)</f>
-        <v>150</v>
+        <v>270.5</v>
       </c>
     </row>
   </sheetData>
@@ -759,24 +785,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>